<commit_message>
Evidencias dd estudio agregadas
</commit_message>
<xml_diff>
--- a/documentacion/CheckLis.xlsx
+++ b/documentacion/CheckLis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando Hernandez\Desktop\ITQ\6to Semestre\Redes de computadoras\StudyCase\StudyCase\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61447397-0EFB-4A1E-AE77-85077E24B628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB5746D-22BB-4EEB-BF07-3F814391B0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Intructions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
   <si>
     <t>#Tab</t>
   </si>
@@ -400,6 +400,27 @@
   </si>
   <si>
     <t>2 ?</t>
+  </si>
+  <si>
+    <t>Hamachi y multiuser</t>
+  </si>
+  <si>
+    <t>Primera topologia</t>
+  </si>
+  <si>
+    <t>Topologia acabada</t>
+  </si>
+  <si>
+    <t>Llamada de meet</t>
+  </si>
+  <si>
+    <t>Prueba ruta flotante</t>
+  </si>
+  <si>
+    <t>Git log</t>
+  </si>
+  <si>
+    <t>Hamachi David</t>
   </si>
 </sst>
 </file>
@@ -1532,6 +1553,326 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2178</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>631645</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>12337</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED3E4F77-3EF8-144F-C837-2486FDFCA23A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="36476" t="51748" r="37163" b="6817"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1569721" y="6618515"/>
+          <a:ext cx="2980781" cy="2668451"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>693420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>811530</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>55245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3AC5007-ACA0-6F3C-B2CC-02BD9BD40D35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1478280" y="3048000"/>
+          <a:ext cx="5612130" cy="2905125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1807028</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>403134</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{420070F3-2D79-AE56-97D5-D1148CD36C27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8077199" y="3058886"/>
+          <a:ext cx="5116649" cy="3570514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1817913</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>118108</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>173082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9957ED9B-D255-F171-1F81-2C680F059A6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8088084" y="7162800"/>
+          <a:ext cx="5604510" cy="2284911"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>21772</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>147502</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>32385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F450E2-B6C1-0364-4556-83759C4F0FD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13596258" y="3603171"/>
+          <a:ext cx="5612130" cy="3156585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>685798</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>63953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>128722</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>9695</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69A39BF9-362F-C72C-B6A9-014D9CA92F6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14260284" y="7379153"/>
+          <a:ext cx="6496867" cy="4060542"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1027612</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F19DE4A-DE38-1CD5-B7EC-12B761C7E682}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1567544" y="10058401"/>
+          <a:ext cx="5730239" cy="3581399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4794,7 +5135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
@@ -34264,10 +34605,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B3:I1000"/>
+  <dimension ref="B3:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34277,12 +34618,12 @@
     <col min="10" max="26" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="56" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="18">
         <v>1</v>
       </c>
@@ -34290,7 +34631,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="18">
         <v>2</v>
       </c>
@@ -34298,7 +34639,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="18">
         <v>3</v>
       </c>
@@ -34306,7 +34647,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
         <v>4</v>
       </c>
@@ -34314,7 +34655,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="64" t="s">
         <v>81</v>
       </c>
@@ -34322,70 +34663,99 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B10" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="64" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C13" s="56" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="J15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="17:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="17:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -35325,5 +35695,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>